<commit_message>
new changes in project
</commit_message>
<xml_diff>
--- a/data/output/bro_summary.xlsx
+++ b/data/output/bro_summary.xlsx
@@ -447,13 +447,13 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>14845120.2</v>
+        <v>14890378.1</v>
       </c>
       <c r="E2">
-        <v>-562921.24</v>
+        <v>-514422.25</v>
       </c>
       <c r="F2">
-        <v>-36.82</v>
+        <v>-32.03</v>
       </c>
       <c r="G2">
         <v>517639.77</v>
@@ -470,13 +470,13 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>16732719.2</v>
+        <v>17480718.7</v>
       </c>
       <c r="E3">
-        <v>-2384756.68</v>
+        <v>-1583190.08</v>
       </c>
       <c r="F3">
-        <v>1507.82</v>
+        <v>2758.46</v>
       </c>
       <c r="G3">
         <v>0</v>

</xml_diff>